<commit_message>
add changes to develop
</commit_message>
<xml_diff>
--- a/src/main/resources/DataProvider/ERHireEducation.xlsx
+++ b/src/main/resources/DataProvider/ERHireEducation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HadeelSalameh\Desktop\Adek2\src\main\resources\DataProvider\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HadeelSalameh\Desktop\HigherEducationAuthrizationAutomatedTests\src\main\resources\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF0B74F-7227-4944-ACA5-2BE66BE24C72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E12AB1-E23C-4D0A-A076-ACDCA76E6199}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0309225A-F2C2-404A-A3FE-7C99E1290A3E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{0309225A-F2C2-404A-A3FE-7C99E1290A3E}"/>
   </bookViews>
   <sheets>
     <sheet name="ER" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
   <si>
     <t>Number of ER</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>ertesting2he@gmail.com</t>
+  </si>
+  <si>
+    <t>ishikite@domy.me</t>
   </si>
 </sst>
 </file>
@@ -442,7 +445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97CAB526-49B1-446F-A8D9-9BDEC7D620B0}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -469,10 +472,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E01BFC1-D8F5-4DE3-A01B-3464F818996A}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -514,12 +517,25 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{A494F800-08D9-4B00-B8EA-A8507746F444}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{F3C59443-C3E4-4E48-81D8-80A9812EF308}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{5E0D3F7F-AF9D-4F4B-8962-EEF8CEBE763C}"/>
-    <hyperlink ref="C3" r:id="rId4" xr:uid="{39D42CAE-D4A5-40D8-BFEA-1720EFDD117A}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{7F3BE83E-07FF-4218-AB60-8499EC11CD09}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{B70C37B7-20EE-4526-9C64-D2F21E07C0B2}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{72B85F0B-6457-4B8C-A81B-51BAD4AC0A1F}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{D42E95C7-BD9C-4473-BA4B-C092DC483637}"/>
+    <hyperlink ref="B4" r:id="rId5" xr:uid="{63EAF4C4-A9A7-4FB6-96E0-DE6E59060060}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{E6AB4A7F-4D7D-454A-8A1F-86E4B4F7979C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -530,7 +546,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -549,7 +565,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -605,12 +621,58 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F81929C-81BD-4516-B4AC-BF480C375589}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="25.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{C10DA038-4A5C-41BE-8DF4-4BECE63DD2DB}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{AF466E58-E942-4B2A-8885-F88648872CC3}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{18CE4D49-9876-4F64-B3EA-9650F3DB2F2C}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{B1BE78B8-B5DC-4D3A-8972-8307C3455D62}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add changes to hadeel
</commit_message>
<xml_diff>
--- a/src/main/resources/DataProvider/ERHireEducation.xlsx
+++ b/src/main/resources/DataProvider/ERHireEducation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HadeelSalameh\Desktop\HigherEducationAuthrizationAutomatedTests\src\main\resources\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E12AB1-E23C-4D0A-A076-ACDCA76E6199}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05077F4A-6D29-48C3-AB1C-24C5F3A82B04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{0309225A-F2C2-404A-A3FE-7C99E1290A3E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{0309225A-F2C2-404A-A3FE-7C99E1290A3E}"/>
   </bookViews>
   <sheets>
     <sheet name="ER" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E01BFC1-D8F5-4DE3-A01B-3464F818996A}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -545,7 +545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C4B5B0-52C8-4201-B15D-3ECB0EEB533B}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>